<commit_message>
Updated DEU_grids model - 2025-09-04 13:29
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU_grids/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_DEU_grids/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34F88E09-5B48-47E2-B2E8-679D704B3CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{90EB55AE-A981-41D6-A528-2D0A1B72A34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11477,7 +11477,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E16403-968A-4129-A5D3-E301EEE71F4F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D2B912-52A7-4371-A99B-E661C727B26F}">
   <dimension ref="B2:AI1404"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated DEU_grids model - 2025-09-04 13:40
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU_grids/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_DEU_grids/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90EB55AE-A981-41D6-A528-2D0A1B72A34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4CB2689-9616-4983-BC9E-F919DA55527C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11477,7 +11477,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D2B912-52A7-4371-A99B-E661C727B26F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C1195D-A4E2-4D1D-95C6-C77BBD1949A8}">
   <dimension ref="B2:AI1404"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>